<commit_message>
Implementazione jx:if per casistiche colore
</commit_message>
<xml_diff>
--- a/src/main/resources/ticket/excel/ticket_template.xlsx
+++ b/src/main/resources/ticket/excel/ticket_template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Java\Workspace\ExcelFromXMLObject\src\main\resources\ticket\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1457BBB3-FF1D-4B16-91FB-01DDE7B8F085}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDB9D3F-5BFB-46F5-999D-31293D5ACF32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="705" windowWidth="28800" windowHeight="15495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Areas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>jx:each(lastCell="F15" items="daAssegnare" var="entry" direction="DOWN")</t>
+          <t>jx:each(lastCell="F15" items="daAssegnare" var="entry" direction="DOWN")
+jx:if(condition="entry.urgenza.equalsIgnoreCase('urgente')" lastCell="F4" areas=["Areas!A7:F7", "A4:F4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('alta')" lastCell="F4" areas=["Areas!A10:F10", "A4:F4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('media')" lastCell="F4" areas=["Areas!A13:F13", "A4:F4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('bassa')" lastCell="F4" areas=["Areas!A16:F16", "A4:F4"])</t>
         </r>
       </text>
     </comment>
@@ -71,8 +76,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">jx:each(lastCell="M15" items="assegnato" var="entry" direction="DOWN")
-</t>
+          <t>jx:each(lastCell="M15" items="assegnato" var="entry" direction="DOWN")
+jx:if(condition="entry.urgenza.equalsIgnoreCase('urgente')" lastCell="M4" areas=["Areas!A7:F7", "H4:M4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('alta')" lastCell="M4" areas=["Areas!A10:F10", "H4:M4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('media')" lastCell="M4" areas=["Areas!A13:F13", "H4:M4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('bassa')" lastCell="M4" areas=["Areas!A16:F16", "H4:M4"])</t>
         </r>
       </text>
     </comment>
@@ -85,8 +93,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">jx:each(lastCell="T15" items="inCorso" var="entry" direction="DOWN")
-</t>
+          <t>jx:each(lastCell="T15" items="inCorso" var="entry" direction="DOWN")
+jx:if(condition="entry.urgenza.equalsIgnoreCase('urgente')" lastCell="T4" areas=["Areas!A7:F7", "O4:T4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('alta')" lastCell="T4" areas=["Areas!A10:F10", "O4:T4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('media')" lastCell="T4" areas=["Areas!A13:F13", "O4:T4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('bassa')" lastCell="T4" areas=["Areas!A16:F16", "O4:T4"])</t>
         </r>
       </text>
     </comment>
@@ -99,8 +110,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">jx:each(lastCell="AA15" items="daTestare" var="entry" direction="DOWN")
-</t>
+          <t>jx:each(lastCell="AA15" items="daTestare" var="entry" direction="DOWN")
+jx:if(condition="entry.urgenza.equalsIgnoreCase('urgente')" lastCell="AA4" areas=["Areas!A7:F7", "V4:AA4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('alta')" lastCell="AA4" areas=["Areas!A10:F10", "V4:AA4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('media')" lastCell="AA4" areas=["Areas!A13:F13", "V4:AA4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('bassa')" lastCell="AA4" areas=["Areas!A16:F16", "V4:AA4"])</t>
         </r>
       </text>
     </comment>
@@ -113,8 +127,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">jx:each(lastCell="AH15" items="daRilasciare" var="entry" direction="DOWN")
-</t>
+          <t>jx:each(lastCell="AH15" items="daRilasciare" var="entry" direction="DOWN")
+jx:if(condition="entry.urgenza.equalsIgnoreCase('urgente')" lastCell="AH4" areas=["Areas!A7:F7", "AC4:AH4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('alta')" lastCell="AH4" areas=["Areas!A10:F10", "AC4:AH4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('media')" lastCell="AH4" areas=["Areas!A13:F13", "AC4:AH4"])
+jx:if(condition="entry.urgenza.equalsIgnoreCase('bassa')" lastCell="AH4" areas=["Areas!A16:F16", "AC4:AH4"])</t>
         </r>
       </text>
     </comment>
@@ -253,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
   <si>
     <t>Ticket Demo</t>
   </si>
@@ -292,6 +309,18 @@
   </si>
   <si>
     <t>${entry.data}</t>
+  </si>
+  <si>
+    <t>Urgente</t>
+  </si>
+  <si>
+    <t>Alta</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Bassa</t>
   </si>
 </sst>
 </file>
@@ -302,7 +331,7 @@
     <numFmt numFmtId="164" formatCode="##\%"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy;@"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,8 +382,47 @@
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Lato UI"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -388,6 +456,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -484,7 +570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -537,22 +623,20 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -837,7 +921,7 @@
   <dimension ref="A1:AH37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1287,11 +1371,6 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
-      <formula>"TODAY()"</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -1313,4 +1392,77 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF5D2E6-9352-4AB1-8773-4BD67A816B32}">
+  <dimension ref="A4:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="4" spans="1:6" ht="21">
+      <c r="A4" s="34" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="42" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="40" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="37"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="37"/>
+      <c r="F13" s="37"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="41" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="38"/>
+      <c r="B16" s="38"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>